<commit_message>
updated dataabase class with load methods to inistialise system
</commit_message>
<xml_diff>
--- a/MScProperties/Bug Log.xlsx
+++ b/MScProperties/Bug Log.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Bug Log</t>
   </si>
@@ -34,15 +37,149 @@
   <si>
     <t>Testing DateConversion class, when invoking dateToCalendar(Date date), I was getting a compiler error due to Null Pointer Exception, this was because when I was converting the utilDate to Calendar, I was assigning a Calendar field a null value and then trying to invoke the Calendar.setTime(Date date) method on the Calendar instance which contained a null value, this was causing the nullPointer exception because I am trying to invoke a method on a Null value, to fix this bug I had to assign a value to the Calendar instance before I could invoke Calendar.setTime(Date date), so instead of assigning a null value assigned the calendar instance the return value from invoking Calendar.getInstance() which returns an instance of the current date/time.</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testing Database class, when loading title - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">com.mysql.jdbc.exceptions.jdbc4.MySQLSyntaxErrorException: Unknown column 'current' in 'field list' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- amended configuration of Element class to include current field, and forgot to add column to MySQL 'title' table</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testing Database class, when loading modifications - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">com.mysql.jdbc.exceptions.jdbc4.MySQLSyntaxErrorException: Table 'msc_properties.titlemodifications' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>doesn't exist - was using modifications class for all modifications then amended design and createdmodification classes for all modifications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testing Database class, when loading modifications - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">com.mysql.jdbc.exceptions.jdbc4.MySQLSyntaxErrorException: Unknown column 'MR' in 'where clause' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- I believe the bug was due to testing method with no data in MySQL database and was using a where clause to return the modifications for specific title 'MR' but there was no records with code='MR'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testing Database class, when creatingModification - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">com.mysql.jdbc.exceptions.jdbc4.MySQLSyntaxErrorException: Unknown column 'modifiedByDate' in 'field list' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- was refering to the column 'modifiedDate' as 'modifiedByDate' within SQL query</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testing Database class, when creatingModification - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">java.sql.SQLException: Field 'modifiedByRef' doesn't have a default value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- forgot to set modifiedByRef column in MySQL table titleModifications to auto incremental, so no value was assigned to the table when trying to execute insert statement</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,8 +214,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -356,7 +521,7 @@
   <dimension ref="A1:B65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,28 +550,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TESTING Database class after implementation of Note class for each Object
</commit_message>
<xml_diff>
--- a/MScProperties/Bug Log.xlsx
+++ b/MScProperties/Bug Log.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bug Log</t>
   </si>
@@ -370,7 +370,29 @@
     </r>
   </si>
   <si>
-    <t>Exception in thread "main" java.lang.IndexOutOfBoundsException: Source does not fit in dest - when invoking Application.setTenancy() due to invoking Collections.copy and dest List not having enough space to fit source list. To resolve I amended my code to invoke destList = new ArrayList(sourceList)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exception in thread "main" java.lang.IndexOutOfBoundsException: Source does not fit in dest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - when invoking Application.setTenancy() due to invoking Collections.copy and dest List not having enough space to fit source list. To resolve I amended my code to invoke destList = new ArrayList(sourceList)</t>
+    </r>
+  </si>
+  <si>
+    <t>Modifications and Notes not loading up correctly, when invoking Database.loadModMap() or Database.loadNoteMap(). Only first Modification or Note for object is loading up at System start up. Upon further testing and investigation, I noticed that there was only one Modification or Note being added to the Map, once all modifications had been loaded from the MySQL database, and this was due to adding the object reference or code, that I am loading modifications or notes for, as the Key to the Map, which is meaning only one Note or Map was being added to the Map as the Key for a Map needs to be unique for each record so when adding additional records to the Map with the same Key, I am just overwriting the previous existing Value assigned to the record with the Key.</t>
   </si>
 </sst>
 </file>
@@ -737,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +917,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>